<commit_message>
CSVs with extracted data and XLSX with improvements
</commit_message>
<xml_diff>
--- a/Improvements.xlsx
+++ b/Improvements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal_GIT_repositories\wikipedia_weather\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{173FAD78-1113-4D0B-8C5F-6F32FE1821FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A01BA8E-7FD7-40D2-BB55-D8707911080C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E19B1317-755C-47C2-BCCE-560E300AE2A5}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{E19B1317-755C-47C2-BCCE-560E300AE2A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Completed</t>
   </si>
@@ -55,6 +55,38 @@
   </si>
   <si>
     <t>Go to the first  climate table, not the first collapsible table</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Unify monthly sunshine data</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>When cm is written in the days count we also multiply it by 10</t>
+  </si>
+  <si>
+    <t>Check Zurich as an example. I tshould  happen in rainy and snowy days</t>
+  </si>
+  <si>
+    <t>The records 'Mean daily sunshine hours', 'Percent possible sunshine' are displayed as 'Mean monthly sunshine hours'
+Check [Zurich, Zunyi] as has the 2 fields so we can check it
+Use Freiburg it to compare the mean daily and mean monthly sunshine hours</t>
+  </si>
+  <si>
+    <t>Get data from the</t>
+  </si>
+  <si>
+    <t>https://ghsl.jrc.ec.europa.eu/datasets.php</t>
   </si>
 </sst>
 </file>
@@ -98,13 +130,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -420,7 +458,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E262D9F9-EC90-4805-A22F-68A9CFC8D96C}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -428,17 +466,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="49.77734375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="49.77734375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="76.88671875" style="4" customWidth="1"/>
     <col min="3" max="3" width="12.109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="11.44140625" style="1" customWidth="1"/>
     <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -449,20 +488,63 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B6" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D34" xr:uid="{F408AFC8-F879-41CD-A0AB-3E60C6911CD6}">
+      <formula1>"High,Medium,Low"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>